<commit_message>
Revert "Merge branch 'master' of https://github.com/sichuan-university-se/SoftwareTraining"
This reverts commit e6294d528838da01cf8b46a00b15ae7f2330ed3e, reversing
changes made to 9a8d387ff0a801c555b5ff76f9270fc44e93ca15.
</commit_message>
<xml_diff>
--- a/需求分析与设计/需求分析与设计.xlsx
+++ b/需求分析与设计/需求分析与设计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZYQ\Documents\GitHub\SoftwareTraining\需求分析与设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3438A989-5DCD-4A75-AB0A-AA64FCAC47D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35766AD1-2DB0-45DF-B282-F566C5A49B15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11604" yWindow="2604" windowWidth="10968" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,15 +175,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>对小组提交的阶段性成果进行评分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对小组的项目整体评分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>同学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对学生的项目整体评分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对学生提交的阶段性成果进行评分</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -238,10 +238,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -546,7 +546,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
@@ -554,38 +554,38 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
@@ -593,7 +593,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -605,7 +605,7 @@
       <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
@@ -613,13 +613,13 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -628,8 +628,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
@@ -637,13 +637,13 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -652,28 +652,28 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="2"/>
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -682,21 +682,21 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>37</v>
+      <c r="A22" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="2"/>
       <c r="B23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -705,7 +705,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="2"/>
       <c r="B25" t="s">
         <v>30</v>
       </c>
@@ -714,19 +714,19 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="2"/>
       <c r="B26" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>22</v>
       </c>
@@ -735,7 +735,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="2"/>
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -744,7 +744,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="2"/>
       <c r="B30" t="s">
         <v>25</v>
       </c>

</xml_diff>